<commit_message>
llenar y almacenar datos en excel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -440,101 +440,101 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B2" t="n">
         <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B3" t="n">
         <v>26</v>
       </c>
       <c r="C3" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B4" t="n">
         <v>26</v>
       </c>
       <c r="C4" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B5" t="n">
         <v>26</v>
       </c>
       <c r="C5" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B6" t="n">
         <v>26</v>
       </c>
       <c r="C6" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B7" t="n">
         <v>26</v>
       </c>
       <c r="C7" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B8" t="n">
         <v>26</v>
       </c>
       <c r="C8" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B9" t="n">
         <v>26</v>
       </c>
       <c r="C9" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="B10" t="n">
         <v>26</v>
       </c>
       <c r="C10" t="n">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>